<commit_message>
Masukin format import siswa
</commit_message>
<xml_diff>
--- a/upload/format_import_siswa.xlsx
+++ b/upload/format_import_siswa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="8025"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="8028"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>nama</t>
   </si>
@@ -142,7 +142,16 @@
     <t>Sita</t>
   </si>
   <si>
-    <t>XI.IPS</t>
+    <t>kelas</t>
+  </si>
+  <si>
+    <t>XRPL1</t>
+  </si>
+  <si>
+    <t>XRPL2</t>
+  </si>
+  <si>
+    <t>REKAYASA PERANGKAT LUNAK</t>
   </si>
 </sst>
 </file>
@@ -483,27 +492,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -513,8 +522,11 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,10 +534,13 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,10 +548,13 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -544,10 +562,13 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -555,10 +576,13 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -566,10 +590,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -577,10 +604,13 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -588,10 +618,13 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -599,10 +632,13 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -610,10 +646,13 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -621,10 +660,13 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -632,10 +674,13 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,10 +688,13 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -654,10 +702,13 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -665,10 +716,13 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -676,10 +730,13 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -687,10 +744,13 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -698,10 +758,13 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -709,10 +772,13 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -720,7 +786,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>